<commit_message>
Updated MDI_javalib and pom.xml
</commit_message>
<xml_diff>
--- a/Tox-To-MDI-Template.xlsx
+++ b/Tox-To-MDI-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A6DF1AB-F522-48E6-9E03-B1ED76854C08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF7D0FC-5E9B-49AA-9E6F-20345451EE3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10245" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="106">
   <si>
     <t>Toxicology-To-MDI Template</t>
   </si>
@@ -34,21 +34,33 @@
     <t>File Id</t>
   </si>
   <si>
+    <t>gtri-testevent-jan</t>
+  </si>
+  <si>
     <t>Laboratory</t>
   </si>
   <si>
     <t>Toxicology Lab Name</t>
   </si>
   <si>
+    <t>UF Health Pathology Labs, Forensic Toxicology Laboratory</t>
+  </si>
+  <si>
     <t>Lab Address: Street</t>
   </si>
   <si>
+    <t>4800 SW 35th Drive</t>
+  </si>
+  <si>
     <t>Lab Address: City</t>
   </si>
   <si>
     <t>Lab Address: State</t>
   </si>
   <si>
+    <t>FL</t>
+  </si>
+  <si>
     <t>Lab Address: Zip</t>
   </si>
   <si>
@@ -61,6 +73,9 @@
     <t>Decedent Sex</t>
   </si>
   <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>Decedent DOB</t>
   </si>
   <si>
@@ -94,6 +109,54 @@
     <t>Container</t>
   </si>
   <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>X353256</t>
+  </si>
+  <si>
+    <t>20 mL</t>
+  </si>
+  <si>
+    <t>Urine</t>
+  </si>
+  <si>
+    <t>ZZZ352356</t>
+  </si>
+  <si>
+    <t>5 mL</t>
+  </si>
+  <si>
+    <t>Bile</t>
+  </si>
+  <si>
+    <t>OO352356</t>
+  </si>
+  <si>
+    <t>3 mL</t>
+  </si>
+  <si>
+    <t>Vitreous Humor</t>
+  </si>
+  <si>
+    <t>XXX352356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stomach Contents </t>
+  </si>
+  <si>
+    <t>MM352356</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>DD352356</t>
+  </si>
+  <si>
+    <t>5 g</t>
+  </si>
+  <si>
     <t>Results</t>
   </si>
   <si>
@@ -109,6 +172,39 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Detected</t>
+  </si>
+  <si>
+    <t>Acetylfentanyl</t>
+  </si>
+  <si>
+    <t>&lt;2.5 ng/mL</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>0.145 g/dL</t>
+  </si>
+  <si>
+    <t>0.160 g/dL</t>
+  </si>
+  <si>
+    <t>0.133 g/dL</t>
+  </si>
+  <si>
+    <t>Fentanyl</t>
+  </si>
+  <si>
+    <t>23 ng/mL</t>
+  </si>
+  <si>
+    <t>not tested</t>
+  </si>
+  <si>
+    <t>Gainesville</t>
+  </si>
+  <si>
     <t>All Time should be in the UTC (or Z) time zone</t>
   </si>
   <si>
@@ -118,12 +214,70 @@
     <t>Analyst</t>
   </si>
   <si>
+    <t>Freeman, Alice J.</t>
+  </si>
+  <si>
+    <t>[note - there may be multiple analysts]</t>
+  </si>
+  <si>
     <t>MDI Case Management Number</t>
   </si>
   <si>
     <t>Examination/Autopsy Number</t>
   </si>
   <si>
+    <t>2024-0014</t>
+  </si>
+  <si>
+    <t>Goldberger, Bruce A.</t>
+  </si>
+  <si>
+    <t>Alachua</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Toxicology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Laboratory Case Number</t>
+    </r>
+  </si>
+  <si>
+    <t>Rush</t>
+  </si>
+  <si>
+    <t>R24-00001</t>
+  </si>
+  <si>
+    <t>2024-01-08 5:00 pm</t>
+  </si>
+  <si>
+    <t>2024-01-10 9:00 am</t>
+  </si>
+  <si>
+    <t>2024-01-22</t>
+  </si>
+  <si>
+    <t>2024-001A</t>
+  </si>
+  <si>
+    <t>femoral</t>
+  </si>
+  <si>
     <t>Agency Name</t>
   </si>
   <si>
@@ -151,12 +305,54 @@
     <t>Investigator/Point of Contact</t>
   </si>
   <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>leaked</t>
+  </si>
+  <si>
+    <t>Office of the Medical Examiner, District 8</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>3217 S.W. 47th Avenue</t>
+  </si>
+  <si>
+    <t>Kinsey, Amy M.</t>
+  </si>
+  <si>
+    <t>Camacho, Ricardo</t>
+  </si>
+  <si>
+    <t>Coyne, Thomas M.</t>
+  </si>
+  <si>
+    <t>L/R</t>
+  </si>
+  <si>
+    <t>45 mL</t>
+  </si>
+  <si>
+    <t>Volatiles</t>
+  </si>
+  <si>
+    <t>Comprehensive Drug Screen</t>
+  </si>
+  <si>
+    <t>NPS Screen and Quantitation</t>
+  </si>
+  <si>
     <t>Toxicologist/Certifier (Title)</t>
   </si>
   <si>
     <t>Testing Requested/Performed</t>
   </si>
   <si>
+    <t>[note - letters are often used to distinguish an autopsy from external exam only]</t>
+  </si>
+  <si>
     <t>General Comments</t>
   </si>
   <si>
@@ -167,9 +363,6 @@
   </si>
   <si>
     <t>Specimen Unique Identifier</t>
-  </si>
-  <si>
-    <t>Toxicology Laboratory Case Number</t>
   </si>
 </sst>
 </file>
@@ -351,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -393,6 +586,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -415,14 +609,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,12 +908,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +926,7 @@
   <dimension ref="A1:J102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +973,9 @@
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -791,23 +987,25 @@
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -819,9 +1017,11 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -833,9 +1033,11 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -847,9 +1049,11 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -861,9 +1065,11 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="B9" s="11">
+        <v>32608</v>
+      </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -874,8 +1080,8 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>32</v>
+      <c r="A10" s="40" t="s">
+        <v>77</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="14"/>
@@ -888,10 +1094,12 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="23"/>
+      <c r="A11" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>88</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -902,10 +1110,12 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="24"/>
+      <c r="A12" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>90</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -916,10 +1126,12 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="23"/>
+      <c r="A13" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>58</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -930,10 +1142,12 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="23"/>
+      <c r="A14" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -944,10 +1158,12 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="23"/>
+      <c r="A15" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>89</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -958,10 +1174,12 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="23"/>
+      <c r="A16" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="24">
+        <v>32608</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -972,10 +1190,12 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="17"/>
+      <c r="A17" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>93</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -986,10 +1206,12 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="17"/>
+      <c r="A18" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1001,7 +1223,7 @@
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="10"/>
@@ -1014,10 +1236,12 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="20"/>
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>71</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1028,10 +1252,12 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="16"/>
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1042,10 +1268,12 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="22"/>
+      <c r="A22" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1056,11 +1284,15 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>101</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1070,10 +1302,12 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="5"/>
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1084,10 +1318,12 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="3">
+        <v>28561</v>
+      </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1098,10 +1334,12 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="18"/>
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -1112,10 +1350,12 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="21"/>
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>74</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -1126,11 +1366,15 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1140,10 +1384,12 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="18"/>
+      <c r="A29" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>67</v>
+      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1155,124 +1401,202 @@
     </row>
     <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="37" t="s">
-        <v>45</v>
+      <c r="I30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="16"/>
+      <c r="G31" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="B32" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="16"/>
+      <c r="G32" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="B33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="16"/>
+      <c r="G33" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="12"/>
+      <c r="B34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="16"/>
+      <c r="G34" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="D35" s="11"/>
-      <c r="E35" s="22"/>
+      <c r="E35" s="22" t="s">
+        <v>95</v>
+      </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="16"/>
+      <c r="G35" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
+      <c r="E36" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="16"/>
+      <c r="G36" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>86</v>
+      </c>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="31"/>
+      <c r="A37" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -1284,7 +1608,9 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="16" t="s">
+        <v>97</v>
+      </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -1296,7 +1622,9 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -1309,22 +1637,22 @@
     </row>
     <row r="41" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1333,10 +1661,18 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="12"/>
+      <c r="B42" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="7"/>
       <c r="H42" s="1"/>
@@ -1345,10 +1681,16 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="11"/>
+      <c r="B43" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="7"/>
       <c r="H43" s="1"/>
@@ -1357,10 +1699,18 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="12"/>
+      <c r="B44" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="7"/>
       <c r="H44" s="1"/>
@@ -1369,10 +1719,16 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="11"/>
+      <c r="B45" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="7"/>
       <c r="H45" s="1"/>
@@ -1381,10 +1737,18 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="12"/>
+      <c r="B46" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="F46" s="1"/>
       <c r="G46" s="7"/>
       <c r="H46" s="1"/>
@@ -1393,10 +1757,18 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="12"/>
+      <c r="B47" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="7"/>
       <c r="H47" s="1"/>
@@ -1405,10 +1777,16 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="11"/>
+      <c r="B48" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="12"/>
+      <c r="E48" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="7"/>
       <c r="H48" s="1"/>
@@ -1417,8 +1795,12 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="11"/>
+      <c r="B49" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="12"/>
@@ -1429,8 +1811,12 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="11"/>
+      <c r="B50" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="12"/>
@@ -1441,8 +1827,12 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="11"/>
+      <c r="B51" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="12"/>
@@ -1452,18 +1842,18 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
+      <c r="A52" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="28"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
@@ -1478,18 +1868,18 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
+      <c r="A54" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="28"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>

</xml_diff>

<commit_message>
Fixed the dob formatting issue on tox-to-mdi.
</commit_message>
<xml_diff>
--- a/Tox-To-MDI-Template.xlsx
+++ b/Tox-To-MDI-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F449467F-594B-4206-8E92-269F4EFFDB58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A53A74-3AF6-432E-9B35-B7398522F712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{E8544DCA-7A15-AA41-9C58-6AD37A29F235}"/>
   </bookViews>
@@ -687,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA2219E-2D71-C14E-8DCA-8D5B763E483A}">
-  <dimension ref="A1:J1048570"/>
+  <dimension ref="A1:J1046452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,6 +763,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="29"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -1401,8 +1402,8 @@
       <c r="I51" s="22"/>
       <c r="J51" s="23"/>
     </row>
-    <row r="1048570" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G1048570" s="2"/>
+    <row r="1046452" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G1046452" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
ADDED RANGE_LOW and RANGE_HIGH
</commit_message>
<xml_diff>
--- a/Tox-To-MDI-Template.xlsx
+++ b/Tox-To-MDI-Template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mriley7/workspace/raven-import-and-submit-api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A53A74-3AF6-432E-9B35-B7398522F712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0AFADC-9385-BB4E-9CA1-7A8D04FF9E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{E8544DCA-7A15-AA41-9C58-6AD37A29F235}"/>
+    <workbookView xWindow="-32980" yWindow="1660" windowWidth="30240" windowHeight="17840" xr2:uid="{E8544DCA-7A15-AA41-9C58-6AD37A29F235}"/>
   </bookViews>
   <sheets>
-    <sheet name="Han Solo" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Note Content</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -81,60 +78,9 @@
     <t>Specimens</t>
   </si>
   <si>
-    <t>Name of Certifier</t>
-  </si>
-  <si>
-    <t>Date of Report Issuance</t>
-  </si>
-  <si>
-    <t>Date/Time of Specimen Collection</t>
-  </si>
-  <si>
-    <t>ME/C Case Notes</t>
-  </si>
-  <si>
-    <t>Decedent DOB</t>
-  </si>
-  <si>
-    <t>Decedent Sex</t>
-  </si>
-  <si>
-    <t>MDI Case Number</t>
-  </si>
-  <si>
-    <t>MDI Case System</t>
-  </si>
-  <si>
-    <t>Decedent Name</t>
-  </si>
-  <si>
     <t>Decedent</t>
   </si>
   <si>
-    <t>Performer</t>
-  </si>
-  <si>
-    <t>Laboratory Case Number</t>
-  </si>
-  <si>
-    <t>Lab Address: Zip</t>
-  </si>
-  <si>
-    <t>Lab Address: State</t>
-  </si>
-  <si>
-    <t>Lab Address: County</t>
-  </si>
-  <si>
-    <t>Lab Address: City</t>
-  </si>
-  <si>
-    <t>Lab Address: Street</t>
-  </si>
-  <si>
-    <t>Toxicology Lab Name</t>
-  </si>
-  <si>
     <t>Laboratory</t>
   </si>
   <si>
@@ -148,13 +94,19 @@
   </si>
   <si>
     <t>General Comments</t>
+  </si>
+  <si>
+    <t>Range Low</t>
+  </si>
+  <si>
+    <t>Range High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +145,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -346,12 +305,25 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -364,14 +336,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,30 +663,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA2219E-2D71-C14E-8DCA-8D5B763E483A}">
-  <dimension ref="A1:J1046452"/>
+  <dimension ref="A1:J1046482"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
-    <col min="9" max="13" width="25.69921875" style="1" customWidth="1"/>
+    <col min="9" max="13" width="25.6640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.69921875" style="1"/>
+    <col min="15" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="15"/>
@@ -722,9 +698,9 @@
       <c r="I1" s="15"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="15"/>
@@ -736,8 +712,8 @@
       <c r="I2" s="15"/>
       <c r="J2" s="17"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -747,51 +723,49 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+        <v>21</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -801,11 +775,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="9"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -815,11 +787,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -829,10 +799,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -842,11 +811,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="9"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -856,11 +823,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="9"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -870,11 +835,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="18"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -884,11 +847,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="9"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -898,9 +859,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="15"/>
@@ -912,11 +873,9 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="18"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -926,11 +885,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="18"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -940,11 +897,9 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="18"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -954,11 +909,9 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="18"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -968,11 +921,9 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="14"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -982,11 +933,9 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="9"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -996,11 +945,9 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="20"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1010,11 +957,9 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="20"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1024,11 +969,9 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="20"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="14"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1038,11 +981,9 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="9"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1052,111 +993,111 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="9"/>
       <c r="C30" s="12"/>
       <c r="D30" s="9"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1168,249 +1109,611 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="2"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="2"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="2"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="27"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="2"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="2"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="2"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="2"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="27"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="2"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="27"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="2"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="27"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="2"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="27"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="2"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="27"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="2"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="27"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="7" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+    </row>
+    <row r="78" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-    </row>
-    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="23"/>
-    </row>
-    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="23"/>
-    </row>
-    <row r="1046452" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G1046452" s="2"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+    </row>
+    <row r="79" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="34"/>
+      <c r="J79" s="35"/>
+    </row>
+    <row r="80" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="30"/>
+    </row>
+    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="30"/>
+    </row>
+    <row r="1046482" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G1046482" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B51:J51"/>
+    <mergeCell ref="B81:J81"/>
     <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="B79:J79"/>
+    <mergeCell ref="B80:J80"/>
     <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>